<commit_message>
Add query wms p/o to sdk Add ack p/o receive to sdk Add ack p/o process to sdk
Add test for above.
</commit_message>
<xml_diff>
--- a/payload/wms connector/purchase order/purchase order mapping.xlsx
+++ b/payload/wms connector/purchase order/purchase order mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="Po header" sheetId="4" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Sheet2" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Po header'!$A$1:$I$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Po header'!$B$1:$K$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Po item'!$D$1:$D$16</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="127">
   <si>
     <t>column type</t>
   </si>
@@ -38,6 +38,9 @@
     <t>wms column name</t>
   </si>
   <si>
+    <t xml:space="preserve">public </t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
@@ -51,6 +54,9 @@
   </si>
   <si>
     <t>as '{header}. ',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { get; set; }</t>
   </si>
   <si>
     <r>
@@ -461,9 +467,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -524,12 +530,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF505050"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF3B4151"/>
@@ -537,11 +537,37 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -552,8 +578,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -569,44 +603,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -614,7 +610,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -628,8 +624,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -644,6 +641,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -652,7 +657,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -660,12 +665,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -715,187 +721,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -924,24 +930,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -953,32 +941,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1000,9 +962,53 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1029,10 +1035,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1041,133 +1047,133 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1232,16 +1238,16 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1592,433 +1598,520 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A$1:A$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85185185185185" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.5740740740741" customWidth="1"/>
-    <col min="2" max="2" width="48.5555555555556" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="34.8518518518519" customWidth="1"/>
-    <col min="4" max="4" width="47.5740740740741" customWidth="1"/>
-    <col min="5" max="5" width="23.1388888888889" customWidth="1"/>
-    <col min="6" max="6" width="24.712962962963" customWidth="1"/>
-    <col min="7" max="7" width="40.8518518518519" customWidth="1"/>
-    <col min="8" max="8" width="70.712962962963" style="5" customWidth="1"/>
-    <col min="9" max="9" width="29.287037037037" customWidth="1"/>
-    <col min="10" max="10" width="40.287037037037" customWidth="1"/>
+    <col min="1" max="1" width="8.85185185185185" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5740740740741" customWidth="1"/>
+    <col min="3" max="3" width="48.5555555555556" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="34.8518518518519" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="47.5740740740741" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1388888888889" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="24.712962962963" customWidth="1"/>
+    <col min="8" max="8" width="24.712962962963" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="40.8518518518519" customWidth="1"/>
+    <col min="10" max="10" width="70.712962962963" style="5" customWidth="1"/>
+    <col min="11" max="11" width="29.287037037037" customWidth="1"/>
+    <col min="12" max="12" width="40.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:9">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="4" customFormat="1" spans="2:11">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-    </row>
-    <row r="2" ht="25.15" customHeight="1" spans="1:9">
-      <c r="A2" s="11" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" ht="25.15" customHeight="1" spans="1:11">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="10" t="str">
+        <f>REPLACE(F2,14,1,G2)</f>
+        <v>as '{header}.PoUuid',</v>
+      </c>
+      <c r="J2" s="23" t="str">
+        <f>_xlfn.CONCAT(C2,D2," ",I2)</f>
+        <v>{Helper.TableAllies}.PoUuid as '{header}.PoUuid',</v>
+      </c>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" ht="25.15" customHeight="1" spans="1:11">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="10" t="str">
+        <f>REPLACE(F3,14,1,G3)</f>
+        <v>as '{header}.CentralPoNum',</v>
+      </c>
+      <c r="J3" s="23" t="str">
+        <f>_xlfn.CONCAT(C3,D3," ",I3)</f>
+        <v>{InfoHelper.TableAllies}.CentralPoNum as '{header}.CentralPoNum',</v>
+      </c>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" ht="15" spans="1:11">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="str">
-        <f>REPLACE(E2,14,1,F2)</f>
-        <v>as '{header}.PoUuid',</v>
-      </c>
-      <c r="H2" s="20" t="str">
-        <f>_xlfn.CONCAT(B2,C2," ",G2)</f>
-        <v>{Helper.TableAllies}.PoUuid as '{header}.PoUuid',</v>
-      </c>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" ht="25.15" customHeight="1" spans="1:9">
-      <c r="A3" s="11" t="s">
+      <c r="D4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="G4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="10" t="str">
-        <f>REPLACE(E3,14,1,F3)</f>
-        <v>as '{header}.CentralPoNum',</v>
-      </c>
-      <c r="H3" s="20" t="str">
-        <f>_xlfn.CONCAT(B3,C3," ",G3)</f>
-        <v>{InfoHelper.TableAllies}.CentralPoNum as '{header}.CentralPoNum',</v>
-      </c>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" ht="15" spans="1:9">
-      <c r="A4" s="11" t="s">
+      <c r="I4" s="10" t="str">
+        <f>REPLACE(F4,14,1,G4)</f>
+        <v>as '{header}.CentralDatabaseNum',</v>
+      </c>
+      <c r="J4" s="23" t="str">
+        <f>_xlfn.CONCAT(C4,D4," ",I4)</f>
+        <v>{Helper.TableAllies}.DatabaseNum as '{header}.CentralDatabaseNum',</v>
+      </c>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" ht="15" spans="1:11">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="G5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="10" t="str">
+        <f>REPLACE(F5,14,1,G5)</f>
+        <v>as '{header}.PoNumber',</v>
+      </c>
+      <c r="J5" s="23" t="str">
+        <f>_xlfn.CONCAT(C5,D5," ",I5)</f>
+        <v>{Helper.TableAllies}.PoNum as '{header}.PoNumber',</v>
+      </c>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" ht="15" spans="1:11">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="10" t="str">
-        <f>REPLACE(E4,14,1,F4)</f>
-        <v>as '{header}.CentralDatabaseNum',</v>
-      </c>
-      <c r="H4" s="20" t="str">
-        <f>_xlfn.CONCAT(B4,C4," ",G4)</f>
-        <v>{Helper.TableAllies}.DatabaseNum as '{header}.CentralDatabaseNum',</v>
-      </c>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" ht="15" spans="1:9">
-      <c r="A5" s="11" t="s">
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="10" t="str">
+        <f>REPLACE(F6,14,1,G6)</f>
+        <v>as '{header}.VendorName',</v>
+      </c>
+      <c r="J6" s="23" t="str">
+        <f>_xlfn.CONCAT(C6,D6," ",I6)</f>
+        <v>{Helper.TableAllies}.VendorName as '{header}.VendorName',</v>
+      </c>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" ht="15" spans="1:11">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="10" t="str">
-        <f>REPLACE(E5,14,1,F5)</f>
-        <v>as '{header}.PoNumber',</v>
-      </c>
-      <c r="H5" s="20" t="str">
-        <f>_xlfn.CONCAT(B5,C5," ",G5)</f>
-        <v>{Helper.TableAllies}.PoNum as '{header}.PoNumber',</v>
-      </c>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" ht="15" spans="1:9">
-      <c r="A6" s="11" t="s">
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" ht="25.15" customHeight="1" spans="1:11">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="10" t="str">
-        <f>REPLACE(E6,14,1,F6)</f>
-        <v>as '{header}.VendorName',</v>
-      </c>
-      <c r="H6" s="20" t="str">
-        <f>_xlfn.CONCAT(B6,C6," ",G6)</f>
-        <v>{Helper.TableAllies}.VendorName as '{header}.VendorName',</v>
-      </c>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" ht="15" spans="1:9">
-      <c r="A7" s="11" t="s">
+      <c r="B8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="10" t="str">
+        <f t="shared" ref="I8:I36" si="0">REPLACE(F8,14,1,G8)</f>
+        <v>as '{header}.PoDate',</v>
+      </c>
+      <c r="J8" s="23" t="str">
+        <f t="shared" ref="J8:J36" si="1">_xlfn.CONCAT(C8,D8," ",I8)</f>
+        <v>{Helper.TableAllies}.PoDate as '{header}.PoDate',</v>
+      </c>
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" ht="15" spans="1:11">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" ht="25.15" customHeight="1" spans="1:9">
-      <c r="A8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="10" t="str">
-        <f t="shared" ref="G8:G36" si="0">REPLACE(E8,14,1,F8)</f>
-        <v>as '{header}.PoDate',</v>
-      </c>
-      <c r="H8" s="20" t="str">
-        <f t="shared" ref="H8:H36" si="1">_xlfn.CONCAT(B8,C8," ",G8)</f>
-        <v>{Helper.TableAllies}.PoDate as '{header}.PoDate',</v>
-      </c>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" ht="15" spans="1:9">
-      <c r="A9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="10" t="str">
+        <v>10</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.CancelAfterDate',</v>
       </c>
-      <c r="H9" s="20" t="str">
+      <c r="J9" s="23" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.CancelDate as '{header}.CancelAfterDate',</v>
       </c>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" ht="15" spans="1:9">
-      <c r="A10" s="11" t="s">
+      <c r="K9" s="11"/>
+    </row>
+    <row r="10" ht="15" spans="1:11">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>9</v>
+      <c r="C10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="10" t="str">
+        <v>10</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="10" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.Terms',</v>
       </c>
-      <c r="H10" s="20" t="str">
+      <c r="J10" s="23" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.Terms as '{header}.Terms',</v>
       </c>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" ht="15" spans="1:9">
-      <c r="A11" s="11" t="s">
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" ht="15" spans="1:11">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>9</v>
+      <c r="C11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="10" t="str">
+        <v>10</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="10" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.WarehousCode',</v>
       </c>
-      <c r="H11" s="20" t="str">
+      <c r="J11" s="23" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.WarehousCode as '{header}.WarehousCode',</v>
       </c>
-      <c r="I11" s="11"/>
-    </row>
-    <row r="12" ht="15" spans="1:9">
-      <c r="A12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" ht="15" spans="1:11">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="22"/>
       <c r="F12" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="10" t="str">
+        <v>10</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="10" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.RequestShipDate',</v>
       </c>
-      <c r="H12" s="20" t="str">
+      <c r="J12" s="23" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.EtaShipDate as '{header}.RequestShipDate',</v>
       </c>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="13" ht="25.15" customHeight="1" spans="1:9">
-      <c r="A13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" ht="25.15" customHeight="1" spans="1:11">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="10" t="str">
+        <v>10</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="10" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.ArrivalDueDate',</v>
       </c>
-      <c r="H13" s="20" t="str">
+      <c r="J13" s="23" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.EtaArrivalDate as '{header}.ArrivalDueDate',</v>
       </c>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" ht="14.45" customHeight="1" spans="1:9">
-      <c r="A14" s="11" t="s">
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" ht="14.45" customHeight="1" spans="1:11">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>9</v>
+      <c r="C14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="10" t="str">
+        <v>10</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="10" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.PublicNote',</v>
       </c>
-      <c r="H14" s="20" t="str">
+      <c r="J14" s="23" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.PublicNote as '{header}.PublicNote',</v>
       </c>
-      <c r="I14" s="11"/>
-    </row>
-    <row r="15" ht="15" spans="1:9">
-      <c r="A15" s="11" t="s">
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" ht="15" spans="1:11">
+      <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>9</v>
+      <c r="C15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="10" t="str">
+        <v>10</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="10" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.PrivateNote',</v>
       </c>
-      <c r="H15" s="20" t="str">
+      <c r="J15" s="23" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.PrivateNote as '{header}.PrivateNote',</v>
       </c>
-      <c r="I15" s="11"/>
+      <c r="K15" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I15">
+  <autoFilter ref="B1:K15">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2031,14 +2124,14 @@
   <sheetPr/>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C$1:E$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85185185185185" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.5740740740741" customWidth="1"/>
-    <col min="2" max="2" width="30.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="30.8888888888889" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="18.5740740740741" customWidth="1"/>
     <col min="4" max="4" width="29.712962962963" customWidth="1"/>
     <col min="5" max="5" width="20.8888888888889" customWidth="1"/>
@@ -2068,21 +2161,23 @@
       <c r="H1" s="6"/>
     </row>
     <row r="2" s="5" customFormat="1" spans="1:8">
-      <c r="A2" s="7"/>
+      <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="B2" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="G2" s="7" t="str">
         <f>REPLACE(E2,5,1,F2)</f>
@@ -2095,19 +2190,19 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G3" s="7" t="str">
         <f>REPLACE(E3,5,1,F3)</f>
@@ -2120,20 +2215,20 @@
     </row>
     <row r="4" ht="15.95" customHeight="1" spans="1:8">
       <c r="A4" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G4" s="8" t="str">
         <f>REPLACE(E4,5,1,F4)</f>
@@ -2146,20 +2241,20 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G5" s="8" t="str">
         <f t="shared" ref="G4:G16" si="0">REPLACE(E5,5,1,F5)</f>
@@ -2172,20 +2267,20 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G6" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2198,22 +2293,22 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G7" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2226,20 +2321,20 @@
     </row>
     <row r="8" ht="25.2" spans="1:8">
       <c r="A8" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2252,20 +2347,20 @@
     </row>
     <row r="9" ht="25.2" spans="1:8">
       <c r="A9" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2278,20 +2373,20 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G10" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2304,22 +2399,22 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2332,20 +2427,20 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G12" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2358,22 +2453,22 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2387,20 +2482,20 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G14" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2413,22 +2508,22 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G15" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2441,20 +2536,20 @@
     </row>
     <row r="16" ht="25.2" spans="1:8">
       <c r="A16" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G16" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2490,223 +2585,223 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2731,131 +2826,131 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add columns to P/O
</commit_message>
<xml_diff>
--- a/payload/wms connector/purchase order/purchase order mapping.xlsx
+++ b/payload/wms connector/purchase order/purchase order mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420"/>
+    <workbookView windowWidth="23040" windowHeight="9420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Po header" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="125">
   <si>
     <t>column type</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Terms</t>
   </si>
   <si>
-    <t>erp add to po header？</t>
-  </si>
-  <si>
     <t>WarehousCode</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>HumanAdjustQty</t>
   </si>
   <si>
-    <t>not exist(CancelledQty?)</t>
-  </si>
-  <si>
     <t>EnterDateUtc</t>
   </si>
   <si>
@@ -467,8 +461,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
@@ -544,7 +538,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -558,19 +559,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -586,31 +588,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -626,7 +606,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -657,7 +644,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -673,7 +660,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -681,7 +668,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -721,13 +715,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,169 +853,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -930,6 +924,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -941,6 +944,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -962,17 +976,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -985,15 +988,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1035,10 +1029,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1047,133 +1041,133 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1600,8 +1594,8 @@
   <sheetPr/>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F$1:F$1048576"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85185185185185" defaultRowHeight="14.4"/>
@@ -1712,7 +1706,7 @@
       </c>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" ht="15" spans="1:11">
+    <row r="4" ht="37.8" spans="1:11">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1747,7 +1741,7 @@
       </c>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" ht="15" spans="1:11">
+    <row r="5" ht="37.8" spans="1:11">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1780,7 +1774,7 @@
       </c>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" ht="15" spans="1:11">
+    <row r="6" ht="37.8" spans="1:11">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1871,7 +1865,7 @@
       </c>
       <c r="K8" s="11"/>
     </row>
-    <row r="9" ht="15" spans="1:11">
+    <row r="9" ht="37.8" spans="1:11">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1904,7 +1898,7 @@
       </c>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" ht="15" spans="1:11">
+    <row r="10" ht="37.8" spans="1:11">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1917,9 +1911,7 @@
       <c r="D10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>28</v>
-      </c>
+      <c r="E10" s="21"/>
       <c r="F10" s="10" t="s">
         <v>10</v>
       </c>
@@ -1939,7 +1931,7 @@
       </c>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" ht="15" spans="1:11">
+    <row r="11" ht="37.8" spans="1:11">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1950,16 +1942,16 @@
         <v>7</v>
       </c>
       <c r="D11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>29</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>30</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="19" t="s">
         <v>11</v>
@@ -1974,7 +1966,7 @@
       </c>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" ht="15" spans="1:11">
+    <row r="12" ht="37.8" spans="1:11">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1985,14 +1977,14 @@
         <v>7</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="19" t="s">
         <v>11</v>
@@ -2018,14 +2010,14 @@
         <v>7</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="19" t="s">
         <v>11</v>
@@ -2051,16 +2043,16 @@
         <v>7</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>36</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="19" t="s">
         <v>11</v>
@@ -2075,7 +2067,7 @@
       </c>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" ht="15" spans="1:11">
+    <row r="15" ht="37.8" spans="1:11">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2086,16 +2078,16 @@
         <v>7</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>11</v>
@@ -2124,8 +2116,8 @@
   <sheetPr/>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:E$1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H$1:H$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85185185185185" defaultRowHeight="14.4"/>
@@ -2134,10 +2126,10 @@
     <col min="2" max="2" width="30.8888888888889" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="18.5740740740741" customWidth="1"/>
     <col min="4" max="4" width="29.712962962963" customWidth="1"/>
-    <col min="5" max="5" width="20.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="20.8888888888889" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="32.4259259259259" customWidth="1"/>
-    <col min="7" max="7" width="35.287037037037" customWidth="1"/>
-    <col min="8" max="8" width="62.712962962963" customWidth="1"/>
+    <col min="7" max="7" width="35.287037037037" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="62.712962962963" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:8">
@@ -2165,19 +2157,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="7" t="str">
         <f>REPLACE(E2,5,1,F2)</f>
@@ -2193,16 +2185,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="G3" s="7" t="str">
         <f>REPLACE(E3,5,1,F3)</f>
@@ -2218,17 +2210,17 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="8" t="str">
         <f>REPLACE(E4,5,1,F4)</f>
@@ -2241,20 +2233,20 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="8" t="str">
         <f t="shared" ref="G4:G16" si="0">REPLACE(E5,5,1,F5)</f>
@@ -2270,17 +2262,17 @@
         <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2296,19 +2288,19 @@
         <v>12</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>51</v>
-      </c>
       <c r="E7" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2324,17 +2316,17 @@
         <v>23</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2350,17 +2342,17 @@
         <v>23</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2376,17 +2368,17 @@
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2402,19 +2394,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2430,17 +2422,17 @@
         <v>12</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G12" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2456,19 +2448,19 @@
         <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>60</v>
-      </c>
       <c r="E13" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2485,17 +2477,17 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2511,19 +2503,19 @@
         <v>12</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2539,17 +2531,17 @@
         <v>23</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G16" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2585,223 +2577,223 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2826,131 +2818,131 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>